<commit_message>
move J-TRP and other motif definitions to a file in the motifs directory
</commit_message>
<xml_diff>
--- a/tests/summary statistics.xlsx
+++ b/tests/summary statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digger\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FB4C62-4D3C-4EC9-9A22-02B1F44F54CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAE982A-1991-44F7-AFA0-EEAC44CF496C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{47B2FD00-D0C8-4089-9FE6-05002D405212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Recorded differences between Digger and IMGT annotation - v0.60.2, 3 October 2023</t>
   </si>
@@ -95,9 +95,6 @@
     <t>IMGT: gene reported in reverse sense</t>
   </si>
   <si>
-    <t>Sequences not annotated by IMGT in this assembly but marked as ORF/P in other sources</t>
-  </si>
-  <si>
     <t>IGLV</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>IMGT reports as functional with non-canonical length of L-PART2 (14 nt)</t>
   </si>
   <si>
-    <t>IMGT reports as functional with non-canonical J-motif</t>
-  </si>
-  <si>
     <t>TOTALS</t>
   </si>
   <si>
@@ -168,6 +162,9 @@
   </si>
   <si>
     <t>Stop codon after position 104</t>
+  </si>
+  <si>
+    <t>Sequences notidentified by Watson et al. in this assembly but marked as ORF/P in other sources</t>
   </si>
 </sst>
 </file>
@@ -525,7 +522,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +546,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -652,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -691,7 +688,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -708,7 +705,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -722,7 +719,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>43</v>
@@ -737,21 +734,21 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -765,7 +762,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>41</v>
@@ -783,12 +780,12 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -802,7 +799,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>13</v>
@@ -816,7 +813,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -828,12 +825,12 @@
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -848,12 +845,12 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -867,7 +864,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -885,41 +882,38 @@
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>2</v>
-      </c>
-      <c r="M22" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <f>SUM(B5:B22)</f>
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C24">
         <f>SUM(C5:C22)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <f>SUM(D5:D22)</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E24">
         <f t="shared" ref="E24:L24" si="0">SUM(E5:E22)</f>
@@ -951,12 +945,12 @@
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1002,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1019,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="M30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1065,12 +1059,12 @@
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -1087,7 +1081,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34">
         <v>52</v>
@@ -1107,7 +1101,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35">
         <v>6</v>
@@ -1124,7 +1118,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <f>SUM(B28:B35)</f>

</xml_diff>

<commit_message>
Fix issue with locus in dig_sequence
</commit_message>
<xml_diff>
--- a/tests/summary statistics.xlsx
+++ b/tests/summary statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\digger\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB6B142-23EE-48A1-9F66-56C736E4AE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA687391-138A-4065-B2B9-9C8747457AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{47B2FD00-D0C8-4089-9FE6-05002D405212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Recorded differences between Digger and IMGT annotation - v0.60.2, 3 October 2023</t>
   </si>
@@ -135,14 +135,61 @@
   </si>
   <si>
     <t>GRAND TOTALS</t>
+  </si>
+  <si>
+    <t>Functional in IMGT and Digger</t>
+  </si>
+  <si>
+    <t>Functional in IMGT only</t>
+  </si>
+  <si>
+    <t>Functional in Digger only</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Analysis of differences</t>
+  </si>
+  <si>
+    <t>non-annotation differences</t>
+  </si>
+  <si>
+    <t>LEADER</t>
+  </si>
+  <si>
+    <t>STOP-CODON</t>
+  </si>
+  <si>
+    <t>RSS</t>
+  </si>
+  <si>
+    <t>Sequence not identified</t>
+  </si>
+  <si>
+    <t>Human IG, TR</t>
+  </si>
+  <si>
+    <t>Rhesus Macaque IG</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -170,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -181,6 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBB8AAA-078D-4BAC-A9C0-37B8575CCDAC}">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
@@ -1000,7 +1048,7 @@
         <v>10</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f>SUM(E23:E30)</f>
         <v>5</v>
       </c>
       <c r="F32">
@@ -1135,6 +1183,163 @@
       </c>
       <c r="D43">
         <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47">
+        <f>B19</f>
+        <v>239</v>
+      </c>
+      <c r="C47">
+        <f>B32</f>
+        <v>233</v>
+      </c>
+      <c r="D47">
+        <f>B47+C47</f>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48">
+        <f>C19</f>
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <f>C32</f>
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:D49" si="3">B48+C48</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49">
+        <f>D19</f>
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <f>D32</f>
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51">
+        <f>E19</f>
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <f>E32</f>
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:D55" si="4">B51+C51</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52">
+        <f>F19</f>
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <f>F32</f>
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53">
+        <f>G19</f>
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <f>G32</f>
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54">
+        <f>H19</f>
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <f>H32</f>
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55">
+        <f>I19</f>
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <f>I32</f>
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1142,5 +1347,6 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>